<commit_message>
Add readme for random noise cancellation
</commit_message>
<xml_diff>
--- a/megaavr/extras/testCases/randomNoiseCancellation/results.xlsx
+++ b/megaavr/extras/testCases/randomNoiseCancellation/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnbra\Documents\School\F2022\SER401\DxCore\megaavr\extras\testCases\randomNoiseCancellation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA96D39B-7B7A-4005-8773-47B90294DEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7542D34-1C1D-40E6-946C-14C988423AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-2865" windowWidth="29040" windowHeight="15990" tabRatio="780" firstSheet="2" activeTab="10" xr2:uid="{8352D553-33B7-4ABD-816F-84F7EDED182C}"/>
+    <workbookView xWindow="23880" yWindow="-2865" windowWidth="29040" windowHeight="15990" tabRatio="790" xr2:uid="{8352D553-33B7-4ABD-816F-84F7EDED182C}"/>
   </bookViews>
   <sheets>
     <sheet name="No noise" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="2">
   <si>
     <t>Average reading:</t>
   </si>
@@ -121,6 +121,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No noise</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1391,6 +1416,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>0.3V</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> with 128-sample accumulation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5201,6 +5256,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>0.3V noise with no accumulation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13211,16 +13291,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13295,16 +13375,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13549,16 +13629,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13973,8 +14053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3665406F-0408-4E39-82FB-6CB93CDA9E43}">
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16085,7 +16165,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BB9340-95EC-4BB1-8538-6A08B8E1795A}">
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22424,7 +22506,7 @@
   <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>